<commit_message>
LV Contacts Regression Suite - 21 June 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0019251_VerifyBasicUIOfContactsOnSFLightning.xlsx
+++ b/TestData/TMTC0019251_VerifyBasicUIOfContactsOnSFLightning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70EB602-8704-4267-A559-7F195F338451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C302DC-8697-49AD-87BE-62F6B9128DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Users</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>PDC Sample</t>
+  </si>
+  <si>
+    <t>Admin User</t>
+  </si>
+  <si>
+    <t>Indrajeet Singh</t>
   </si>
 </sst>
 </file>
@@ -460,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,14 +477,20 @@
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -491,7 +503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238E81D2-2BA2-4C65-87A5-507061E9159C}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Contacts Final Merge - 19 Mar 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTC0019251_VerifyBasicUIOfContactsOnSFLightning.xlsx
+++ b/TestData/TMTC0019251_VerifyBasicUIOfContactsOnSFLightning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C302DC-8697-49AD-87BE-62F6B9128DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F5D3B9-6033-40BE-B91B-05D58F3AA621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Users</t>
   </si>
@@ -67,9 +67,6 @@
     <t>ListViewValues</t>
   </si>
   <si>
-    <t>All Contacts</t>
-  </si>
-  <si>
     <t>External Contact List</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>Recently Viewed Contacts</t>
   </si>
   <si>
-    <t>Recently Viewed</t>
-  </si>
-  <si>
     <t>James Craven</t>
   </si>
   <si>
@@ -128,6 +122,9 @@
   </si>
   <si>
     <t>Indrajeet Singh</t>
+  </si>
+  <si>
+    <t>Added By Einstein</t>
   </si>
 </sst>
 </file>
@@ -468,7 +465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -482,15 +479,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -501,10 +498,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238E81D2-2BA2-4C65-87A5-507061E9159C}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,42 +516,37 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -637,37 +629,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -689,17 +681,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>